<commit_message>
Conflitos checados. Novas regras adicionadas.
</commit_message>
<xml_diff>
--- a/info/queoperadora.xlsx
+++ b/info/queoperadora.xlsx
@@ -190,9 +190,6 @@
     <t>Amazonia</t>
   </si>
   <si>
-    <t>6057-6060, 6193-6199, 6370-6499, 7099, 71-75, 95</t>
-  </si>
-  <si>
     <t>71,72 e 95</t>
   </si>
   <si>
@@ -259,33 +256,20 @@
     <t>Desativada</t>
   </si>
   <si>
+    <t xml:space="preserve">VERMELHO - Conflito de regras </t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">6100-6193, 6299,65,6651-6799,68,6999,7971-7999,80, </t>
+      <t xml:space="preserve">6057-6060, </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>8814-8899</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">6310-6339, 6589-6599, 7052-7062, 76, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8800-8999</t>
+      <t>6182-6199</t>
     </r>
     <r>
       <rPr>
@@ -295,18 +279,113 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, 91 a 94</t>
+      <t>, 6370-6499, 7099, 71-75, 95</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">VERMELHO - Conflito de regras </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6300-6339</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 6589-6599, 7052-7062, 76, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8800-8899</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 91 a 94,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6168-6181</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6100-6167</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6200-6300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,65,6651-6799,68,6999,7971-7999,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8010-8099</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -349,6 +428,12 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1037,12 +1122,12 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -1050,7 +1135,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
@@ -1058,7 +1143,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
@@ -1066,7 +1151,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>51</v>
@@ -1074,7 +1159,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>51</v>
@@ -1090,7 +1175,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>51</v>
@@ -1098,7 +1183,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>22</v>
@@ -1114,15 +1199,15 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>51</v>
@@ -1131,7 +1216,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1144,15 +1228,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="2" max="2" width="37.1640625" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="4" width="47.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.5" customWidth="1"/>
@@ -1172,10 +1256,10 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1189,13 +1273,13 @@
         <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
         <v>51</v>
@@ -1238,7 +1322,7 @@
         <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1249,10 +1333,10 @@
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
@@ -1272,10 +1356,10 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
@@ -1301,7 +1385,7 @@
         <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
         <v>51</v>
@@ -1349,22 +1433,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
         <v>51</v>
@@ -1372,7 +1456,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -1389,13 +1473,12 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Conflitos resolvidos. Versão 0.01 beta
</commit_message>
<xml_diff>
--- a/info/queoperadora.xlsx
+++ b/info/queoperadora.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="260" windowWidth="8600" windowHeight="12840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operadoras, Padrão" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
   <si>
     <t>Amazônia (91 a 99)</t>
   </si>
@@ -163,9 +163,6 @@
     <t>São Paulo</t>
   </si>
   <si>
-    <t>9911-9939</t>
-  </si>
-  <si>
     <t>Pelotas e Região</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
   </si>
   <si>
     <t>Minas Gerais</t>
-  </si>
-  <si>
-    <t>96,9960-9979 e 9991-9999</t>
   </si>
   <si>
     <t>84,85 e 86</t>
@@ -380,12 +374,51 @@
       <t>8010-8099</t>
     </r>
   </si>
+  <si>
+    <t>9911-9920</t>
+  </si>
+  <si>
+    <t>95-99</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>AZUL - Novas Regras ou regras corrigidas</t>
+  </si>
+  <si>
+    <t>LARANJA - Regras nao utilizadas</t>
+  </si>
+  <si>
+    <t>11.19</t>
+  </si>
+  <si>
+    <t>91.99</t>
+  </si>
+  <si>
+    <t>61.69</t>
+  </si>
+  <si>
+    <t>21.28</t>
+  </si>
+  <si>
+    <t>81.89</t>
+  </si>
+  <si>
+    <t>51.55</t>
+  </si>
+  <si>
+    <t>31.38</t>
+  </si>
+  <si>
+    <t>71.79</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -433,6 +466,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF6600"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -489,13 +528,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1122,12 +1164,12 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -1135,7 +1177,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
@@ -1143,7 +1185,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
@@ -1151,18 +1193,18 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1170,20 +1212,20 @@
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>22</v>
@@ -1194,23 +1236,23 @@
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1226,254 +1268,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
         <v>81</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
         <v>65</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>95</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7">
+      <c r="F10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8">
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9">
-        <v>95</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novas modificacoes e melhoras para no módulo python
</commit_message>
<xml_diff>
--- a/info/queoperadora.xlsx
+++ b/info/queoperadora.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="95">
   <si>
     <t>Amazônia (91 a 99)</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>71.79</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>96-99</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -538,6 +544,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1270,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1281,7 +1290,7 @@
     <col min="3" max="3" width="37.1640625" customWidth="1"/>
     <col min="4" max="4" width="60.33203125" customWidth="1"/>
     <col min="5" max="5" width="47.33203125" customWidth="1"/>
-    <col min="6" max="6" width="55.6640625" customWidth="1"/>
+    <col min="6" max="6" width="63.83203125" customWidth="1"/>
     <col min="7" max="7" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1335,8 +1344,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3">
-        <v>53</v>
+      <c r="A3" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>47</v>
@@ -1470,6 +1479,9 @@
       </c>
       <c r="E8" t="s">
         <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>94</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>

</xml_diff>